<commit_message>
Merged anuradha n manali code all working
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/Pythoncode.xlsx
+++ b/src/test/resources/Exceldata/Pythoncode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65a12dafce843d13/Desktop/DS_Algo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{374C2964-11FA-47B1-9248-11F0D6F4A4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71749DA5-2F61-4AD1-8B14-4E2EB2CC9080}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{374C2964-11FA-47B1-9248-11F0D6F4A4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F95B37D-560B-42F8-B5FD-96233057449E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{421A814B-9063-40BF-BBE4-2E6FA14044A4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{421A814B-9063-40BF-BBE4-2E6FA14044A4}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCode" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>print 'hello';</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>print 'Hey';</t>
   </si>
@@ -48,9 +45,6 @@
   </si>
   <si>
     <t>System.out.println("Hi Java");</t>
-  </si>
-  <si>
-    <t>System.out.println("Hey Java");</t>
   </si>
 </sst>
 </file>
@@ -413,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF9E08D-B3D1-4699-861A-C10D17E82A30}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,27 +420,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Anu(2) + manali code merged
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/Pythoncode.xlsx
+++ b/src/test/resources/Exceldata/Pythoncode.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65a12dafce843d13/Desktop/DS_Algo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirti\git\numpy_coders\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{374C2964-11FA-47B1-9248-11F0D6F4A4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F95B37D-560B-42F8-B5FD-96233057449E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B937857-D6D9-4264-9B7B-BA9AB6C6C2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{421A814B-9063-40BF-BBE4-2E6FA14044A4}"/>
   </bookViews>
@@ -38,13 +38,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>print 'Hey';</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
     <t>System.out.println("Hi Java");</t>
+  </si>
+  <si>
+    <t>print 'Hey Selenium';</t>
   </si>
 </sst>
 </file>
@@ -104,10 +104,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,7 +406,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,17 +416,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>